<commit_message>
add building test caces
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/VisitorData.xlsx
+++ b/src/test/resources/testData/VisitorData.xlsx
@@ -4,20 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="17244" windowHeight="8220" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="17244" windowHeight="8220" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="visitorManage" sheetId="1" r:id="rId1"/>
     <sheet name="CheckedOut" sheetId="2" r:id="rId2"/>
     <sheet name="CheckInVisitors" sheetId="3" r:id="rId3"/>
+    <sheet name="CheckedIn" sheetId="4" r:id="rId4"/>
+    <sheet name="Overdue" sheetId="5" r:id="rId5"/>
+    <sheet name="manageBuilding" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:G27"/>
+  <oleSize ref="A1:Q27"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>admin</t>
   </si>
@@ -131,6 +134,42 @@
   </si>
   <si>
     <t>nimal@gmail.com</t>
+  </si>
+  <si>
+    <t>visitor_NIC</t>
+  </si>
+  <si>
+    <t>6348445764v</t>
+  </si>
+  <si>
+    <t>7821459632v</t>
+  </si>
+  <si>
+    <t>4578963245v</t>
+  </si>
+  <si>
+    <t>5612345783v</t>
+  </si>
+  <si>
+    <t>8695748612v</t>
+  </si>
+  <si>
+    <t>BuildingName</t>
+  </si>
+  <si>
+    <t>floorName</t>
+  </si>
+  <si>
+    <t>buildingNo1</t>
+  </si>
+  <si>
+    <t>buildingNo2</t>
+  </si>
+  <si>
+    <t>floorNo1</t>
+  </si>
+  <si>
+    <t>floorNo2</t>
   </si>
 </sst>
 </file>
@@ -582,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
@@ -754,4 +793,112 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add testcases for functions
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/VisitorData.xlsx
+++ b/src/test/resources/testData/VisitorData.xlsx
@@ -15,12 +15,12 @@
     <sheet name="manageBuilding" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:Q27"/>
+  <oleSize ref="A1:O27"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>admin</t>
   </si>
@@ -170,6 +170,24 @@
   </si>
   <si>
     <t>floorNo2</t>
+  </si>
+  <si>
+    <t>NewBuildingName</t>
+  </si>
+  <si>
+    <t>building6</t>
+  </si>
+  <si>
+    <t>building10</t>
+  </si>
+  <si>
+    <t>NewFloorname</t>
+  </si>
+  <si>
+    <t>floorNo12</t>
+  </si>
+  <si>
+    <t>FloorNo5</t>
   </si>
 </sst>
 </file>
@@ -864,38 +882,60 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19.109375" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test cases for manage staff
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/VisitorData.xlsx
+++ b/src/test/resources/testData/VisitorData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="17244" windowHeight="8220" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="18432" windowHeight="8220" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="visitorManage" sheetId="1" r:id="rId1"/>
@@ -17,19 +17,16 @@
     <sheet name="SystemUser" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:Q27"/>
+  <oleSize ref="A1:I27"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="87">
   <si>
     <t>admin</t>
   </si>
   <si>
-    <t>recep</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -54,12 +51,6 @@
     <t>5665555545V</t>
   </si>
   <si>
-    <t>dnjnf</t>
-  </si>
-  <si>
-    <t>vnkjvhv</t>
-  </si>
-  <si>
     <t>staffMember</t>
   </si>
   <si>
@@ -289,6 +280,9 @@
   </si>
   <si>
     <t>6956445321v</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -646,7 +640,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -659,10 +653,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -675,18 +669,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>123</v>
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -710,26 +704,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -766,143 +760,143 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>112453542</v>
       </c>
       <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>33</v>
       </c>
-      <c r="I2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" t="s">
-        <v>36</v>
-      </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M2">
         <v>245565665656</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="O2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>112453542</v>
       </c>
       <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="H3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>31</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>32</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>33</v>
       </c>
-      <c r="I3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" t="s">
-        <v>36</v>
-      </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M3">
         <v>245565665656</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="O3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -931,22 +925,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -969,17 +963,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1005,44 +999,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
         <v>49</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1071,60 +1065,60 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" t="s">
-        <v>65</v>
-      </c>
       <c r="G2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
@@ -1135,28 +1129,28 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="F3" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>0</v>
@@ -1180,7 +1174,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1198,81 +1192,81 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G2">
         <v>123</v>
       </c>
       <c r="H2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G3">
         <v>123</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I3" s="5"/>
     </row>

</xml_diff>